<commit_message>
beginning template for all data
</commit_message>
<xml_diff>
--- a/Customers/Customers.xlsx
+++ b/Customers/Customers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Brick</t>
   </si>
   <si>
-    <t>Weinacht</t>
-  </si>
-  <si>
     <t>Hansen</t>
   </si>
   <si>
@@ -64,12 +61,6 @@
     <t>Eqpt. Max</t>
   </si>
   <si>
-    <t>Silas (up)</t>
-  </si>
-  <si>
-    <t>Silas (down)</t>
-  </si>
-  <si>
     <t>Riggert</t>
   </si>
   <si>
@@ -182,6 +173,15 @@
   </si>
   <si>
     <t>Good looking plots</t>
+  </si>
+  <si>
+    <t>Silas</t>
+  </si>
+  <si>
+    <t>Weinact</t>
+  </si>
+  <si>
+    <t>shape = 0</t>
   </si>
 </sst>
 </file>
@@ -553,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -566,8 +566,8 @@
     <col min="5" max="5" width="9.44140625" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
@@ -575,80 +575,84 @@
     <col min="14" max="14" width="8.33203125" customWidth="1"/>
     <col min="15" max="15" width="6.6640625" style="7" customWidth="1"/>
     <col min="16" max="17" width="6.33203125" customWidth="1"/>
-    <col min="18" max="18" width="7" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="T1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="U1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>2016</v>
@@ -689,7 +693,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O2" s="7">
         <v>0.43</v>
@@ -700,20 +704,23 @@
       <c r="Q2" s="4">
         <v>-6.4000000000000001E-2</v>
       </c>
-      <c r="R2" s="7">
-        <v>0</v>
+      <c r="R2" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="S2" s="7">
         <v>0</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="7">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
         <v>0.17</v>
       </c>
-      <c r="U2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -749,7 +756,7 @@
         <v>0.25</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L25" si="1">I3/H3</f>
+        <f t="shared" ref="L3:L24" si="1">I3/H3</f>
         <v>0.87121212121212122</v>
       </c>
       <c r="M3" s="3">
@@ -757,7 +764,7 @@
         <v>0.25</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O3" s="7">
         <v>6.8000000000000005E-2</v>
@@ -768,22 +775,25 @@
       <c r="Q3" s="4">
         <v>-0.11</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="7">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="S3" s="7">
+      <c r="T3" s="7">
         <v>2E-3</v>
       </c>
-      <c r="T3" s="10">
+      <c r="U3" s="10">
         <v>0.69</v>
       </c>
-      <c r="U3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>2017</v>
@@ -824,7 +834,7 @@
         <v>0.5</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O4" s="7">
         <v>0.22</v>
@@ -835,22 +845,25 @@
       <c r="Q4" s="4">
         <v>0.41</v>
       </c>
-      <c r="R4" s="7">
-        <v>0.46</v>
+      <c r="R4" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="S4" s="7">
         <v>0.46</v>
       </c>
-      <c r="T4" s="10">
+      <c r="T4" s="7">
+        <v>0.46</v>
+      </c>
+      <c r="U4" s="10">
         <v>14.8</v>
       </c>
-      <c r="U4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>2017</v>
@@ -892,7 +905,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O5" s="7">
         <v>0.1</v>
@@ -903,22 +916,25 @@
       <c r="Q5" s="4">
         <v>0.37</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S5" s="7">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="S5" s="7">
+      <c r="T5" s="7">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="T5" s="3">
+      <c r="U5" s="3">
         <v>1.43</v>
       </c>
-      <c r="U5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
         <v>2017</v>
@@ -959,7 +975,7 @@
         <v>0.5</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O6" s="7">
         <v>0.47</v>
@@ -970,20 +986,23 @@
       <c r="Q6" s="4">
         <v>-1.03</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S6" s="7">
         <v>0.89</v>
       </c>
-      <c r="S6" s="7">
+      <c r="T6" s="7">
         <v>0.9</v>
       </c>
-      <c r="T6" s="3">
+      <c r="U6" s="3">
         <v>8.4499999999999993</v>
       </c>
-      <c r="U6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1016,13 +1035,13 @@
         <v>0.88</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M7" s="3">
         <v>0.2</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O7" s="7">
         <v>0.55000000000000004</v>
@@ -1033,22 +1052,23 @@
       <c r="Q7" s="4">
         <v>-0.31</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="4"/>
+      <c r="S7" s="7">
         <v>0.06</v>
       </c>
-      <c r="S7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="T7" s="3">
+      <c r="T7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="U7" s="3">
         <v>1.3</v>
       </c>
-      <c r="U7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>2017</v>
@@ -1089,7 +1109,7 @@
         <v>0.5</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O8" s="7">
         <v>0.16</v>
@@ -1100,22 +1120,23 @@
       <c r="Q8" s="4">
         <v>-0.3</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="4"/>
+      <c r="S8" s="7">
         <v>0.64</v>
       </c>
-      <c r="S8" s="7">
+      <c r="T8" s="7">
         <v>0.62</v>
       </c>
-      <c r="T8" s="3">
+      <c r="U8" s="3">
         <v>9.75</v>
       </c>
-      <c r="U8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2016</v>
@@ -1156,7 +1177,7 @@
         <v>0.5</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O9" s="7">
         <v>0.05</v>
@@ -1167,19 +1188,20 @@
       <c r="Q9" s="4">
         <v>-0.25</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="4"/>
+      <c r="S9" s="7">
         <v>0.22</v>
       </c>
-      <c r="S9" s="7">
+      <c r="T9" s="7">
         <v>0.27</v>
       </c>
-      <c r="T9" s="3">
+      <c r="U9" s="3">
         <v>2.12</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1">
         <v>2017</v>
@@ -1220,7 +1242,7 @@
         <v>0.25</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="O10" s="7">
         <v>0.05</v>
@@ -1231,22 +1253,23 @@
       <c r="Q10" s="4">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="4"/>
+      <c r="S10" s="7">
         <v>0.16</v>
       </c>
-      <c r="S10" s="7">
+      <c r="T10" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T10" s="3">
+      <c r="U10" s="3">
         <v>16</v>
       </c>
-      <c r="U10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="11">
         <v>2017</v>
@@ -1287,7 +1310,7 @@
         <v>0.23</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O11" s="15">
         <v>0.27</v>
@@ -1298,22 +1321,23 @@
       <c r="Q11" s="16">
         <v>0.55000000000000004</v>
       </c>
-      <c r="R11" s="15">
+      <c r="R11" s="16"/>
+      <c r="S11" s="15">
         <v>0.11</v>
       </c>
-      <c r="S11" s="15">
+      <c r="T11" s="15">
         <v>0.12</v>
       </c>
-      <c r="T11" s="14">
+      <c r="U11" s="14">
         <v>4.96</v>
       </c>
-      <c r="U11" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V11" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="13">
         <v>2016</v>
@@ -1354,7 +1378,7 @@
         <v>0.15</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O12" s="15">
         <v>0.13</v>
@@ -1365,19 +1389,20 @@
       <c r="Q12" s="16">
         <v>0.25600000000000001</v>
       </c>
-      <c r="R12" s="15">
-        <v>0.01</v>
-      </c>
+      <c r="R12" s="16"/>
       <c r="S12" s="15">
         <v>0.01</v>
       </c>
-      <c r="T12" s="14">
+      <c r="T12" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="U12" s="14">
         <v>1.02</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13" s="11">
         <v>2017</v>
@@ -1389,7 +1414,7 @@
         <v>42916</v>
       </c>
       <c r="E13" s="11">
-        <f>D13-C13</f>
+        <f t="shared" ref="E13:E24" si="2">D13-C13</f>
         <v>29</v>
       </c>
       <c r="F13" s="11">
@@ -1418,7 +1443,7 @@
         <v>0.6</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O13" s="15">
         <v>0.03</v>
@@ -1429,17 +1454,18 @@
       <c r="Q13" s="16">
         <v>0.76</v>
       </c>
-      <c r="R13" s="15">
-        <v>0.17</v>
-      </c>
+      <c r="R13" s="16"/>
       <c r="S13" s="15">
         <v>0.17</v>
       </c>
-      <c r="T13" s="14">
+      <c r="T13" s="15">
+        <v>0.17</v>
+      </c>
+      <c r="U13" s="14">
         <v>46.5</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1453,7 +1479,7 @@
         <v>42634</v>
       </c>
       <c r="E14" s="1">
-        <f>D14-C14</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="F14" s="1">
@@ -1482,7 +1508,7 @@
         <v>0.2</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O14" s="7">
         <v>4.4999999999999998E-2</v>
@@ -1493,19 +1519,20 @@
       <c r="Q14" s="4">
         <v>0.12</v>
       </c>
-      <c r="R14" s="7">
+      <c r="R14" s="4"/>
+      <c r="S14" s="7">
         <v>2E-3</v>
       </c>
-      <c r="S14" s="7">
+      <c r="T14" s="7">
         <v>1E-3</v>
       </c>
-      <c r="T14" s="3">
+      <c r="U14" s="3">
         <v>0.69</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>2016</v>
@@ -1517,7 +1544,7 @@
         <v>42649</v>
       </c>
       <c r="E15" s="1">
-        <f>D15-C15</f>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="F15" s="1">
@@ -1546,7 +1573,7 @@
         <v>0.3</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O15" s="7">
         <v>0.04</v>
@@ -1557,17 +1584,18 @@
       <c r="Q15" s="4">
         <v>0.51</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="4"/>
+      <c r="S15" s="7">
         <v>0.13</v>
       </c>
-      <c r="S15" s="7">
+      <c r="T15" s="7">
         <v>0.18</v>
       </c>
-      <c r="T15" s="3">
+      <c r="U15" s="3">
         <v>5.26</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1581,7 +1609,7 @@
         <v>42642</v>
       </c>
       <c r="E16" s="1">
-        <f>D16-C16</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="F16" s="1">
@@ -1600,13 +1628,13 @@
         <v>0.15</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M16" s="3">
         <v>0.1</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O16" s="7">
         <v>0.21</v>
@@ -1617,22 +1645,23 @@
       <c r="Q16" s="4">
         <v>0.23</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R16" s="4"/>
+      <c r="S16" s="7">
         <v>2E-3</v>
       </c>
-      <c r="S16" s="7" t="s">
+      <c r="T16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="V16" t="s">
         <v>52</v>
       </c>
-      <c r="T16" s="3">
-        <v>0.59</v>
-      </c>
-      <c r="U16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>2017</v>
@@ -1644,7 +1673,7 @@
         <v>42943</v>
       </c>
       <c r="E17" s="1">
-        <f>D17-C17</f>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="F17" s="1">
@@ -1673,7 +1702,7 @@
         <v>0.8</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O17" s="7">
         <v>0.06</v>
@@ -1684,30 +1713,40 @@
       <c r="Q17" s="4">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="R17" s="7">
-        <v>0.6</v>
-      </c>
+      <c r="R17" s="4"/>
       <c r="S17" s="7">
         <v>0.6</v>
       </c>
-      <c r="T17" s="3">
+      <c r="T17" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="U17" s="3">
         <v>9</v>
       </c>
-      <c r="U17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>2016</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="C18" s="5">
+        <v>42578</v>
+      </c>
+      <c r="D18" s="5">
+        <v>42608</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
       <c r="G18" s="1">
         <v>3</v>
       </c>
@@ -1716,53 +1755,127 @@
       </c>
       <c r="I18">
         <v>28.5</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.65</v>
       </c>
       <c r="L18" s="3">
         <f t="shared" si="1"/>
         <v>1.0795454545454546</v>
       </c>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O18" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="P18" s="4">
+        <v>0.34</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="R18" s="4"/>
+      <c r="S18" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="T18" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="U18" s="3">
+        <v>7.48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>2016</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="C19" s="5">
+        <v>42556</v>
+      </c>
+      <c r="D19" s="5">
+        <v>42647</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
       <c r="G19" s="1">
         <v>5</v>
       </c>
       <c r="H19" s="1">
         <v>36.799999999999997</v>
       </c>
-      <c r="L19" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="P19" s="4">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="R19" s="4"/>
+      <c r="S19" s="7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="U19" s="3">
+        <v>1.65</v>
+      </c>
+      <c r="V19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>2016</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="C20" s="5">
+        <v>42552</v>
+      </c>
+      <c r="D20" s="5">
+        <v>42642</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
       <c r="G20" s="1">
         <v>2</v>
       </c>
@@ -1770,57 +1883,132 @@
         <v>18.399999999999999</v>
       </c>
       <c r="I20">
-        <v>19.7</v>
+        <v>17.3</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.93</v>
       </c>
       <c r="L20" s="3">
         <f t="shared" si="1"/>
-        <v>1.0706521739130435</v>
-      </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.94021739130434789</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" s="7">
+        <v>0.09</v>
+      </c>
+      <c r="P20" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="R20" s="4"/>
+      <c r="S20" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="T20" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="U20" s="3">
+        <v>22</v>
+      </c>
+      <c r="V20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B21">
         <v>2016</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="C21" s="5">
+        <v>42556</v>
+      </c>
+      <c r="D21" s="5">
+        <v>42646</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
       <c r="G21" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H21" s="1">
-        <v>18.399999999999999</v>
+        <v>26.4</v>
       </c>
       <c r="I21">
-        <v>17.3</v>
+        <v>19.5</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0.45</v>
       </c>
       <c r="L21" s="3">
         <f t="shared" si="1"/>
-        <v>0.94021739130434789</v>
-      </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.73863636363636365</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21" s="7">
+        <v>0.22</v>
+      </c>
+      <c r="P21" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="R21" s="4"/>
+      <c r="S21" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="T21" s="7">
+        <v>0.09</v>
+      </c>
+      <c r="U21" s="3">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B22">
         <v>2016</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="C22" s="5">
+        <v>42591</v>
+      </c>
+      <c r="D22" s="5">
+        <v>42654</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
       <c r="G22" s="1">
         <v>3</v>
       </c>
@@ -1828,103 +2016,176 @@
         <v>26.4</v>
       </c>
       <c r="I22">
-        <v>19.5</v>
+        <v>33.200000000000003</v>
+      </c>
+      <c r="J22" s="1">
+        <v>60</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.19</v>
       </c>
       <c r="L22" s="3">
         <f t="shared" si="1"/>
-        <v>0.73863636363636365</v>
-      </c>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.2575757575757578</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O22" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="P22" s="4">
+        <v>1.45</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>-0.218</v>
+      </c>
+      <c r="R22" s="4"/>
+      <c r="S22" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="T22" s="7">
+        <v>0.38</v>
+      </c>
+      <c r="U22" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="V22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>2016</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1">
-        <v>4</v>
+      <c r="C23" s="5">
+        <v>42591</v>
+      </c>
+      <c r="D23" s="5">
+        <v>42656</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2.1666599999999998</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
       </c>
       <c r="H23" s="1">
-        <v>36.799999999999997</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="I23">
-        <v>33.200000000000003</v>
+        <v>18.100000000000001</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.32500000000000001</v>
       </c>
       <c r="L23" s="3">
         <f t="shared" si="1"/>
-        <v>0.90217391304347838</v>
-      </c>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.98369565217391319</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="P23" s="4">
+        <v>2.415</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>-1</v>
+      </c>
+      <c r="R23" s="4"/>
+      <c r="S23" s="7">
+        <v>0.59</v>
+      </c>
+      <c r="T23" s="7">
+        <v>0.59</v>
+      </c>
+      <c r="U23" s="3">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B24">
         <v>2016</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24">
+      <c r="C24" s="5">
+        <v>42557</v>
+      </c>
+      <c r="D24" s="5">
+        <v>42647</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1">
         <v>3</v>
       </c>
       <c r="H24" s="1">
         <v>26.4</v>
       </c>
       <c r="I24">
-        <v>18.100000000000001</v>
+        <v>26.7</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.2</v>
       </c>
       <c r="L24" s="3">
         <f t="shared" si="1"/>
-        <v>0.68560606060606066</v>
-      </c>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25">
-        <v>2016</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1">
-        <v>3</v>
-      </c>
-      <c r="H25" s="1">
-        <v>26.4</v>
-      </c>
-      <c r="I25">
-        <v>26.7</v>
-      </c>
-      <c r="L25" s="3">
-        <f t="shared" si="1"/>
         <v>1.0113636363636365</v>
       </c>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
+      <c r="M24" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O24" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="P24" s="4">
+        <v>1.29</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>-0.32</v>
+      </c>
+      <c r="R24" s="4"/>
+      <c r="S24" s="7">
+        <v>0.41</v>
+      </c>
+      <c r="T24" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="U24" s="3">
+        <v>3.08</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:E25">

</xml_diff>